<commit_message>
Day2 using Github clean stuff up
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>LocationName</t>
   </si>
   <si>
     <t>AB</t>
+  </si>
+  <si>
+    <t>BC</t>
   </si>
   <si>
     <t>AssetTypeName</t>
@@ -406,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -417,6 +420,11 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -432,22 +440,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>